<commit_message>
registration no to main
</commit_message>
<xml_diff>
--- a/pdfContent.xlsx
+++ b/pdfContent.xlsx
@@ -14,9 +14,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <x:si>
-    <x:t>Full name</x:t>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+  <x:si>
+    <x:t>Timestamp</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Full name (as per NRIC)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Gender</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Age Group</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Email address</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Contact Number</x:t>
   </x:si>
   <x:si>
     <x:t>Registration No</x:t>
@@ -28,31 +43,85 @@
     <x:t>Adam Tan</x:t>
   </x:si>
   <x:si>
+    <x:t>Male</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21-30</x:t>
+  </x:si>
+  <x:si>
+    <x:t>echen009@e.ntu.edu</x:t>
+  </x:si>
+  <x:si>
     <x:t>Successfully registered! Here is your registration number to the event.</x:t>
   </x:si>
   <x:si>
+    <x:t>Dr. John Williams</x:t>
+  </x:si>
+  <x:si>
+    <x:t>test@abc.com.sg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Allen Wood</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Rebecca Alvarez</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Caden Chen</x:t>
+  </x:si>
+  <x:si>
+    <x:t>31-40</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mark Sanchez</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Barbara Blevins</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Natalie Prince</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Koh Kong Ming</x:t>
+  </x:si>
+  <x:si>
+    <x:t>41-50</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Anthony Harris</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Lisa Chan Ming Ming</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Female</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cody Robinson</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Steven Houston</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jaime Green</x:t>
+  </x:si>
+  <x:si>
     <x:t>Becky Chen</x:t>
   </x:si>
   <x:si>
-    <x:t>Lisa Chan Ming Ming</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Caden Chen</x:t>
+    <x:t>Jean Williams</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kayla Flores</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Amy Navarro</x:t>
   </x:si>
   <x:si>
     <x:t>Danielle Sim</x:t>
   </x:si>
   <x:si>
-    <x:t>Koh Kong Ming</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mark Sanchez</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Jean Williams</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Cody Robinson</x:t>
+    <x:t>Tiffany Martinez</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -98,13 +167,20 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="1">
+  <x:cellStyleXfs count="2">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="22" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="1">
+  <x:cellXfs count="2">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -403,13 +479,13 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:C10"/>
+  <x:dimension ref="A1:H21"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:3">
+    <x:row r="1" spans="1:8">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -419,104 +495,540 @@
       <x:c r="C1" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
-    </x:row>
-    <x:row r="2" spans="1:3">
-      <x:c r="A2" s="0" t="s">
+      <x:c r="D1" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="B2" s="0" t="n">
+      <x:c r="E1" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F1" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="G1" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H1" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:8">
+      <x:c r="A2" s="1">
+        <x:v>45417.8346064815</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F2" s="0" t="n">
+        <x:v>14583376</x:v>
+      </x:c>
+      <x:c r="G2" s="0" t="n">
         <x:v>1001</x:v>
       </x:c>
-      <x:c r="C2" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:3">
-      <x:c r="A3" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="B3" s="0" t="n">
+      <x:c r="H2" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:8">
+      <x:c r="A3" s="1">
+        <x:v>45418.5026388889</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="n">
+        <x:v>30338111</x:v>
+      </x:c>
+      <x:c r="G3" s="0" t="n">
         <x:v>1002</x:v>
       </x:c>
-      <x:c r="C3" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:3">
-      <x:c r="A4" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="n">
+      <x:c r="H3" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:8">
+      <x:c r="A4" s="1">
+        <x:v>45419.7410416667</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F4" s="0" t="n">
+        <x:v>30990800</x:v>
+      </x:c>
+      <x:c r="G4" s="0" t="n">
         <x:v>1003</x:v>
       </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:3">
-      <x:c r="A5" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="B5" s="0" t="n">
+      <x:c r="H4" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:8">
+      <x:c r="A5" s="1">
+        <x:v>45417.7739467593</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="n">
+        <x:v>81218466</x:v>
+      </x:c>
+      <x:c r="G5" s="0" t="n">
         <x:v>1004</x:v>
       </x:c>
-      <x:c r="C5" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:3">
-      <x:c r="A6" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="B6" s="0" t="n">
+      <x:c r="H5" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:8">
+      <x:c r="A6" s="1">
+        <x:v>45418.5026388889</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F6" s="0" t="n">
+        <x:v>22789443</x:v>
+      </x:c>
+      <x:c r="G6" s="0" t="n">
         <x:v>1005</x:v>
       </x:c>
-      <x:c r="C6" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:3">
-      <x:c r="A7" s="0" t="s">
+      <x:c r="H6" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:8">
+      <x:c r="A7" s="1">
+        <x:v>45416.0048842593</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="B7" s="0" t="n">
+      <x:c r="D7" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F7" s="0" t="n">
+        <x:v>26663693</x:v>
+      </x:c>
+      <x:c r="G7" s="0" t="n">
         <x:v>1006</x:v>
       </x:c>
-      <x:c r="C7" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:3">
-      <x:c r="A8" s="0" t="s">
+      <x:c r="H7" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:8">
+      <x:c r="A8" s="1">
+        <x:v>45417.9609143519</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F8" s="0" t="n">
+        <x:v>42910376</x:v>
+      </x:c>
+      <x:c r="G8" s="0" t="n">
+        <x:v>1007</x:v>
+      </x:c>
+      <x:c r="H8" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:8">
+      <x:c r="A9" s="1">
+        <x:v>45417.6209143518</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="E9" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F9" s="0" t="n">
+        <x:v>45345003</x:v>
+      </x:c>
+      <x:c r="G9" s="0" t="n">
+        <x:v>1008</x:v>
+      </x:c>
+      <x:c r="H9" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:8">
+      <x:c r="A10" s="1">
+        <x:v>45418.5249652778</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E10" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F10" s="0" t="n">
+        <x:v>24770454</x:v>
+      </x:c>
+      <x:c r="G10" s="0" t="n">
+        <x:v>1009</x:v>
+      </x:c>
+      <x:c r="H10" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:8">
+      <x:c r="A11" s="1">
+        <x:v>45419.872337963</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E11" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F11" s="0" t="n">
+        <x:v>39467735</x:v>
+      </x:c>
+      <x:c r="G11" s="0" t="n">
+        <x:v>1010</x:v>
+      </x:c>
+      <x:c r="H11" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:8">
+      <x:c r="A12" s="1">
+        <x:v>45416.6572222222</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="B8" s="0" t="n">
-        <x:v>1007</x:v>
-      </x:c>
-      <x:c r="C8" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:3">
-      <x:c r="A9" s="0" t="s">
+      <x:c r="E12" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="B9" s="0" t="n">
-        <x:v>1008</x:v>
-      </x:c>
-      <x:c r="C9" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:3">
-      <x:c r="A10" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="B10" s="0" t="n">
-        <x:v>1009</x:v>
-      </x:c>
-      <x:c r="C10" s="0" t="s">
-        <x:v>4</x:v>
+      <x:c r="F12" s="0" t="n">
+        <x:v>19760685</x:v>
+      </x:c>
+      <x:c r="G12" s="0" t="n">
+        <x:v>1011</x:v>
+      </x:c>
+      <x:c r="H12" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:8">
+      <x:c r="A13" s="1">
+        <x:v>45418.0745138889</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E13" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F13" s="0" t="n">
+        <x:v>28557906</x:v>
+      </x:c>
+      <x:c r="G13" s="0" t="n">
+        <x:v>1012</x:v>
+      </x:c>
+      <x:c r="H13" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:8">
+      <x:c r="A14" s="1">
+        <x:v>45417.5652199074</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="D14" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E14" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F14" s="0" t="n">
+        <x:v>28688027</x:v>
+      </x:c>
+      <x:c r="G14" s="0" t="n">
+        <x:v>1013</x:v>
+      </x:c>
+      <x:c r="H14" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:8">
+      <x:c r="A15" s="1">
+        <x:v>45416.6572222222</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="D15" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E15" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F15" s="0" t="n">
+        <x:v>30279019</x:v>
+      </x:c>
+      <x:c r="G15" s="0" t="n">
+        <x:v>1014</x:v>
+      </x:c>
+      <x:c r="H15" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:8">
+      <x:c r="A16" s="1">
+        <x:v>45418.1527083333</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="E16" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F16" s="0" t="n">
+        <x:v>15480124</x:v>
+      </x:c>
+      <x:c r="G16" s="0" t="n">
+        <x:v>1015</x:v>
+      </x:c>
+      <x:c r="H16" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:8">
+      <x:c r="A17" s="1">
+        <x:v>45417.2744675926</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="C17" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="D17" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="E17" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F17" s="0" t="n">
+        <x:v>27498330</x:v>
+      </x:c>
+      <x:c r="G17" s="0" t="n">
+        <x:v>1016</x:v>
+      </x:c>
+      <x:c r="H17" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:8">
+      <x:c r="A18" s="1">
+        <x:v>45418.8998726852</x:v>
+      </x:c>
+      <x:c r="B18" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="C18" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="D18" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="E18" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F18" s="0" t="n">
+        <x:v>42487189</x:v>
+      </x:c>
+      <x:c r="G18" s="0" t="n">
+        <x:v>1017</x:v>
+      </x:c>
+      <x:c r="H18" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:8">
+      <x:c r="A19" s="1">
+        <x:v>45418.4218171296</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C19" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="E19" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F19" s="0" t="n">
+        <x:v>53416701</x:v>
+      </x:c>
+      <x:c r="G19" s="0" t="n">
+        <x:v>1018</x:v>
+      </x:c>
+      <x:c r="H19" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:8">
+      <x:c r="A20" s="1">
+        <x:v>45419.7410416667</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="C20" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="D20" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E20" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F20" s="0" t="n">
+        <x:v>24219363</x:v>
+      </x:c>
+      <x:c r="G20" s="0" t="n">
+        <x:v>1019</x:v>
+      </x:c>
+      <x:c r="H20" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:8">
+      <x:c r="A21" s="1">
+        <x:v>45418.5249652778</x:v>
+      </x:c>
+      <x:c r="B21" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C21" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="D21" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E21" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F21" s="0" t="n">
+        <x:v>31310453</x:v>
+      </x:c>
+      <x:c r="G21" s="0" t="n">
+        <x:v>1020</x:v>
+      </x:c>
+      <x:c r="H21" s="0" t="s">
+        <x:v>12</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>